<commit_message>
fix and feat: review doc string and organize new function "avalia_estrutura"
</commit_message>
<xml_diff>
--- a/planilhas_teste/pilares.xlsx
+++ b/planilhas_teste/pilares.xlsx
@@ -19,16 +19,16 @@
     <t>Danos</t>
   </si>
   <si>
-    <t>Elemento 1</t>
+    <t>Pilar 1</t>
   </si>
   <si>
-    <t>Elemento 2</t>
+    <t>Pilar 2</t>
   </si>
   <si>
-    <t>Elemento n-1</t>
+    <t>Pilar 3</t>
   </si>
   <si>
-    <t>Elemento n</t>
+    <t>Pilar 4</t>
   </si>
   <si>
     <t>Fi</t>
@@ -116,7 +116,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -134,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -286,6 +286,13 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -331,14 +338,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +666,7 @@
     <col min="9" max="9" style="16" width="8.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +687,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -707,268 +714,136 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9">
-        <v>2</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9">
-        <v>2</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>2</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="9">
-        <v>2</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
-        <v>2</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9">
-        <v>2</v>
-      </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9">
-        <v>2</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="9">
-        <v>2</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="8">
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" s="8">
         <v>1</v>
       </c>
       <c r="I8" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8">
-        <v>1</v>
-      </c>
-      <c r="E10" s="9">
-        <v>2</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9">
-        <v>2</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
-        <v>2</v>
-      </c>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
-      <c r="I11" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -976,173 +851,85 @@
         <v>1</v>
       </c>
       <c r="C12" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
       </c>
       <c r="E12" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>2</v>
-      </c>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9">
-        <v>2</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9">
-        <v>2</v>
-      </c>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
-      <c r="I13" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="8">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="9">
-        <v>2</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
-        <v>2</v>
-      </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9">
-        <v>2</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9">
-        <v>2</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
-        <v>2</v>
-      </c>
-      <c r="H15" s="8">
-        <v>1</v>
-      </c>
-      <c r="I15" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
-        <v>2</v>
-      </c>
-      <c r="D16" s="8">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9">
-        <v>2</v>
-      </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <v>2</v>
-      </c>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-      <c r="C17" s="12">
-        <v>2</v>
-      </c>
-      <c r="D17" s="11">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12">
-        <v>2</v>
-      </c>
-      <c r="F17" s="11">
-        <v>1</v>
-      </c>
-      <c r="G17" s="12">
-        <v>2</v>
-      </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1153,7 +940,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -1164,7 +951,7 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -1175,7 +962,7 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -1186,7 +973,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1197,7 +984,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="13"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -1208,7 +995,7 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1219,7 +1006,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1230,7 +1017,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1241,7 +1028,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1252,7 +1039,7 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="13"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -1263,7 +1050,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -1274,7 +1061,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="13"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1285,7 +1072,7 @@
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>

</xml_diff>